<commit_message>
Clean Version before implementing Double EventList Check
</commit_message>
<xml_diff>
--- a/Reports/New Base_Report_Iteration_2.xlsx
+++ b/Reports/New Base_Report_Iteration_2.xlsx
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1509" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1509" uniqueCount="640">
   <si>
     <t>Regression thread</t>
   </si>
@@ -1931,22 +1931,16 @@
     <t>Triggering State</t>
   </si>
   <si>
-    <t>v1_label(1)</t>
+    <t>v0_label(1)</t>
+  </si>
+  <si>
+    <t>v1_label(2)</t>
   </si>
   <si>
     <t>v1_Severity</t>
   </si>
   <si>
     <t>v1_State</t>
-  </si>
-  <si>
-    <t>v2_label(2)</t>
-  </si>
-  <si>
-    <t>v2_Severity</t>
-  </si>
-  <si>
-    <t>v2_State</t>
   </si>
   <si>
     <t>NExec</t>
@@ -2724,7 +2718,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="42"/>
+        <fgColor indexed="23"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6617,7 +6611,7 @@
         <v>STD ID</v>
       </c>
       <c r="E3" s="175" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="F3" s="149"/>
       <c r="G3" s="157" t="str">
@@ -6625,7 +6619,7 @@
         <v>Written by</v>
       </c>
       <c r="H3" s="185" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="I3" s="138"/>
       <c r="J3" s="139"/>
@@ -6668,7 +6662,7 @@
         <v>Writing date</v>
       </c>
       <c r="H5" s="185" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="I5" s="138"/>
       <c r="J5" s="139"/>
@@ -6931,7 +6925,7 @@
         <v>IO schedule version</v>
       </c>
       <c r="E20" t="s" s="184">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="F20" s="149"/>
       <c r="G20" s="149"/>
@@ -8404,19 +8398,19 @@
         <v>595</v>
       </c>
       <c r="G1" t="s" s="193">
+        <v>581</v>
+      </c>
+      <c r="H1" t="s" s="193">
+        <v>582</v>
+      </c>
+      <c r="I1" t="s" s="193">
         <v>596</v>
       </c>
-      <c r="H1" t="s" s="193">
+      <c r="J1" t="s" s="193">
         <v>597</v>
       </c>
-      <c r="I1" t="s" s="193">
+      <c r="K1" t="s" s="193">
         <v>598</v>
-      </c>
-      <c r="J1" t="s" s="193">
-        <v>599</v>
-      </c>
-      <c r="K1" t="s" s="193">
-        <v>600</v>
       </c>
       <c r="L1" t="s" s="193">
         <v>586</v>
@@ -8446,22 +8440,22 @@
     <row r="2"/>
     <row r="3">
       <c r="A3" t="s">
+        <v>605</v>
+      </c>
+      <c r="B3" t="s">
         <v>607</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>609</v>
       </c>
-      <c r="C3" t="s">
-        <v>611</v>
-      </c>
       <c r="D3" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="E3" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="F3" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="G3" t="n">
         <v>0.0</v>
@@ -8470,26 +8464,26 @@
         <v>27</v>
       </c>
       <c r="I3" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="J3" t="n">
         <v>2.0</v>
       </c>
       <c r="K3" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="L3" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="M3" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="N3" t="s" s="196">
-        <v>601</v>
+        <v>29</v>
       </c>
       <c r="O3" s="197"/>
       <c r="P3" s="197" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="Q3" s="197"/>
       <c r="R3" t="s" s="197">
@@ -8501,22 +8495,22 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>605</v>
+      </c>
+      <c r="B4" t="s">
         <v>607</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>609</v>
       </c>
-      <c r="C4" t="s">
-        <v>611</v>
-      </c>
       <c r="D4" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="E4" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="F4" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="G4" t="n">
         <v>0.0</v>
@@ -8525,26 +8519,26 @@
         <v>27</v>
       </c>
       <c r="I4" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="J4" t="n">
         <v>2.0</v>
       </c>
       <c r="K4" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="L4" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="M4" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="N4" t="s" s="196">
-        <v>601</v>
+        <v>29</v>
       </c>
       <c r="O4" s="197"/>
       <c r="P4" s="197" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="Q4" s="197"/>
       <c r="R4" t="s" s="197">
@@ -8556,22 +8550,22 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>605</v>
+      </c>
+      <c r="B5" t="s">
         <v>607</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>609</v>
       </c>
-      <c r="C5" t="s">
-        <v>611</v>
-      </c>
       <c r="D5" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E5" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="F5" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="G5" t="n">
         <v>0.0</v>
@@ -8580,26 +8574,26 @@
         <v>27</v>
       </c>
       <c r="I5" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="J5" t="n">
         <v>3.0</v>
       </c>
       <c r="K5" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="L5" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="M5" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="N5" t="s" s="196">
-        <v>601</v>
+        <v>29</v>
       </c>
       <c r="O5" s="197"/>
       <c r="P5" s="197" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="Q5" s="197"/>
       <c r="R5" t="s" s="197">
@@ -8611,22 +8605,22 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>605</v>
+      </c>
+      <c r="B6" t="s">
         <v>607</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>609</v>
       </c>
-      <c r="C6" t="s">
-        <v>611</v>
-      </c>
       <c r="D6" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="E6" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="F6" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="G6" t="n">
         <v>0.0</v>
@@ -8635,26 +8629,26 @@
         <v>27</v>
       </c>
       <c r="I6" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="J6" t="n">
         <v>3.0</v>
       </c>
       <c r="K6" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="L6" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="M6" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="N6" t="s" s="196">
-        <v>601</v>
+        <v>29</v>
       </c>
       <c r="O6" s="197"/>
       <c r="P6" s="197" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="Q6" s="197"/>
       <c r="R6" t="s" s="197">
@@ -8666,22 +8660,22 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>605</v>
+      </c>
+      <c r="B7" t="s">
         <v>607</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>609</v>
       </c>
-      <c r="C7" t="s">
-        <v>611</v>
-      </c>
       <c r="D7" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="E7" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="F7" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="G7" t="n">
         <v>0.0</v>
@@ -8690,26 +8684,26 @@
         <v>27</v>
       </c>
       <c r="I7" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="J7" t="n">
         <v>2.0</v>
       </c>
       <c r="K7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="L7" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="M7" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="N7" t="s" s="196">
-        <v>601</v>
+        <v>29</v>
       </c>
       <c r="O7" s="197"/>
       <c r="P7" s="197" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="Q7" s="197"/>
       <c r="R7" t="s" s="197">
@@ -8721,22 +8715,22 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>605</v>
+      </c>
+      <c r="B8" t="s">
         <v>607</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>609</v>
       </c>
-      <c r="C8" t="s">
-        <v>611</v>
-      </c>
       <c r="D8" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="E8" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="F8" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="G8" t="n">
         <v>0.0</v>
@@ -8745,26 +8739,26 @@
         <v>27</v>
       </c>
       <c r="I8" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="J8" t="n">
         <v>2.0</v>
       </c>
       <c r="K8" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="L8" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="M8" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="N8" t="s" s="196">
-        <v>601</v>
+        <v>29</v>
       </c>
       <c r="O8" s="197"/>
       <c r="P8" s="197" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="Q8" s="197"/>
       <c r="R8" t="s" s="197">
@@ -8776,22 +8770,22 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>605</v>
+      </c>
+      <c r="B9" t="s">
         <v>607</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>609</v>
       </c>
-      <c r="C9" t="s">
-        <v>611</v>
-      </c>
       <c r="D9" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E9" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="F9" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="G9" t="n">
         <v>0.0</v>
@@ -8800,26 +8794,26 @@
         <v>27</v>
       </c>
       <c r="I9" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="J9" t="n">
         <v>3.0</v>
       </c>
       <c r="K9" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="L9" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="M9" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="N9" t="s" s="196">
-        <v>601</v>
+        <v>29</v>
       </c>
       <c r="O9" s="197"/>
       <c r="P9" s="197" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="Q9" s="197"/>
       <c r="R9" t="s" s="197">
@@ -8831,22 +8825,22 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>605</v>
+      </c>
+      <c r="B10" t="s">
         <v>607</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>609</v>
       </c>
-      <c r="C10" t="s">
-        <v>611</v>
-      </c>
       <c r="D10" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="E10" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="F10" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="G10" t="n">
         <v>0.0</v>
@@ -8855,26 +8849,26 @@
         <v>27</v>
       </c>
       <c r="I10" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="J10" t="n">
         <v>3.0</v>
       </c>
       <c r="K10" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="L10" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="M10" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="N10" t="s" s="196">
-        <v>601</v>
+        <v>29</v>
       </c>
       <c r="O10" s="197"/>
       <c r="P10" s="197" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="Q10" s="197"/>
       <c r="R10" t="s" s="197">
@@ -8886,22 +8880,22 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>605</v>
+      </c>
+      <c r="B11" t="s">
         <v>607</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>609</v>
       </c>
-      <c r="C11" t="s">
-        <v>611</v>
-      </c>
       <c r="D11" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="E11" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="F11" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="G11" t="n">
         <v>0.0</v>
@@ -8910,26 +8904,26 @@
         <v>27</v>
       </c>
       <c r="I11" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="J11" t="n">
         <v>2.0</v>
       </c>
       <c r="K11" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="L11" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="M11" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="N11" t="s" s="196">
-        <v>601</v>
+        <v>29</v>
       </c>
       <c r="O11" s="197"/>
       <c r="P11" s="197" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="Q11" s="197"/>
       <c r="R11" t="s" s="197">
@@ -8941,22 +8935,22 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>605</v>
+      </c>
+      <c r="B12" t="s">
         <v>607</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>609</v>
       </c>
-      <c r="C12" t="s">
-        <v>611</v>
-      </c>
       <c r="D12" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="E12" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="F12" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="G12" t="n">
         <v>0.0</v>
@@ -8965,26 +8959,26 @@
         <v>27</v>
       </c>
       <c r="I12" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="J12" t="n">
         <v>2.0</v>
       </c>
       <c r="K12" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="L12" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="M12" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="N12" t="s" s="196">
-        <v>601</v>
+        <v>29</v>
       </c>
       <c r="O12" s="197"/>
       <c r="P12" s="197" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="Q12" s="197"/>
       <c r="R12" t="s" s="197">
@@ -9389,1296 +9383,1296 @@
         <v>583</v>
       </c>
       <c r="I1" t="s" s="398">
+        <v>630</v>
+      </c>
+      <c r="K1" t="s" s="399">
+        <v>631</v>
+      </c>
+      <c r="M1" t="s" s="400">
         <v>632</v>
       </c>
-      <c r="K1" t="s" s="399">
+      <c r="O1" t="s" s="401">
         <v>633</v>
       </c>
-      <c r="M1" t="s" s="400">
+      <c r="Q1" t="s" s="402">
         <v>634</v>
       </c>
-      <c r="O1" t="s" s="401">
+      <c r="S1" t="s" s="403">
         <v>635</v>
-      </c>
-      <c r="Q1" t="s" s="402">
-        <v>636</v>
-      </c>
-      <c r="S1" t="s" s="403">
-        <v>637</v>
       </c>
     </row>
     <row r="2">
       <c r="G2" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="H2" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="I2" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="J2" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="K2" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="L2" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="M2" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="N2" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="O2" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="P2" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="Q2" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="R2" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="S2" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="T2" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="s">
+        <v>599</v>
+      </c>
+      <c r="C4" t="s">
+        <v>602</v>
+      </c>
+      <c r="D4" t="s">
+        <v>600</v>
+      </c>
+      <c r="E4" t="s">
         <v>601</v>
       </c>
-      <c r="C4" t="s">
-        <v>604</v>
-      </c>
-      <c r="D4" t="s">
-        <v>602</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>603</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s" s="257">
         <v>605</v>
       </c>
-      <c r="G4" t="s" s="257">
+      <c r="H4" t="s" s="257">
+        <v>606</v>
+      </c>
+      <c r="I4" t="s" s="258">
         <v>607</v>
       </c>
-      <c r="H4" t="s" s="257">
+      <c r="J4" t="s" s="258">
+        <v>606</v>
+      </c>
+      <c r="K4" t="s" s="259">
         <v>608</v>
       </c>
-      <c r="I4" t="s" s="258">
+      <c r="L4" t="s" s="259">
+        <v>606</v>
+      </c>
+      <c r="M4" t="s" s="260">
         <v>609</v>
       </c>
-      <c r="J4" t="s" s="258">
-        <v>608</v>
-      </c>
-      <c r="K4" t="s" s="259">
+      <c r="N4" t="s" s="260">
+        <v>606</v>
+      </c>
+      <c r="O4" t="s" s="261">
         <v>610</v>
       </c>
-      <c r="L4" t="s" s="259">
-        <v>608</v>
-      </c>
-      <c r="M4" t="s" s="260">
+      <c r="P4" t="s" s="261">
+        <v>606</v>
+      </c>
+      <c r="Q4" t="s" s="262">
         <v>611</v>
       </c>
-      <c r="N4" t="s" s="260">
-        <v>608</v>
-      </c>
-      <c r="O4" t="s" s="261">
+      <c r="R4" t="s" s="262">
+        <v>606</v>
+      </c>
+      <c r="S4" t="s" s="263">
         <v>612</v>
       </c>
-      <c r="P4" t="s" s="261">
-        <v>608</v>
-      </c>
-      <c r="Q4" t="s" s="262">
-        <v>613</v>
-      </c>
-      <c r="R4" t="s" s="262">
-        <v>608</v>
-      </c>
-      <c r="S4" t="s" s="263">
-        <v>614</v>
-      </c>
       <c r="T4" t="s" s="263">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
+        <v>599</v>
+      </c>
+      <c r="C5" t="s">
+        <v>602</v>
+      </c>
+      <c r="D5" t="s">
+        <v>600</v>
+      </c>
+      <c r="E5" t="s">
         <v>601</v>
       </c>
-      <c r="C5" t="s">
-        <v>604</v>
-      </c>
-      <c r="D5" t="s">
-        <v>602</v>
-      </c>
-      <c r="E5" t="s">
-        <v>603</v>
-      </c>
       <c r="F5" t="s">
+        <v>614</v>
+      </c>
+      <c r="G5" t="s" s="264">
+        <v>605</v>
+      </c>
+      <c r="H5" t="s" s="264">
+        <v>606</v>
+      </c>
+      <c r="I5" t="s" s="265">
+        <v>607</v>
+      </c>
+      <c r="J5" t="s" s="265">
+        <v>606</v>
+      </c>
+      <c r="K5" t="s" s="266">
+        <v>608</v>
+      </c>
+      <c r="L5" t="s" s="266">
+        <v>606</v>
+      </c>
+      <c r="M5" t="s" s="267">
+        <v>609</v>
+      </c>
+      <c r="N5" t="s" s="267">
+        <v>606</v>
+      </c>
+      <c r="O5" t="s" s="268">
+        <v>610</v>
+      </c>
+      <c r="P5" t="s" s="268">
+        <v>606</v>
+      </c>
+      <c r="Q5" t="s" s="269">
+        <v>615</v>
+      </c>
+      <c r="R5" t="s" s="269">
+        <v>606</v>
+      </c>
+      <c r="S5" t="s" s="270">
         <v>616</v>
       </c>
-      <c r="G5" t="s" s="264">
-        <v>607</v>
-      </c>
-      <c r="H5" t="s" s="264">
-        <v>608</v>
-      </c>
-      <c r="I5" t="s" s="265">
-        <v>609</v>
-      </c>
-      <c r="J5" t="s" s="265">
-        <v>608</v>
-      </c>
-      <c r="K5" t="s" s="266">
-        <v>610</v>
-      </c>
-      <c r="L5" t="s" s="266">
-        <v>608</v>
-      </c>
-      <c r="M5" t="s" s="267">
-        <v>611</v>
-      </c>
-      <c r="N5" t="s" s="267">
-        <v>608</v>
-      </c>
-      <c r="O5" t="s" s="268">
-        <v>612</v>
-      </c>
-      <c r="P5" t="s" s="268">
-        <v>608</v>
-      </c>
-      <c r="Q5" t="s" s="269">
-        <v>617</v>
-      </c>
-      <c r="R5" t="s" s="269">
-        <v>608</v>
-      </c>
-      <c r="S5" t="s" s="270">
-        <v>618</v>
-      </c>
       <c r="T5" t="s" s="270">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C7" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D7" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="E7" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="F7" t="s">
+        <v>603</v>
+      </c>
+      <c r="G7" t="s" s="271">
         <v>605</v>
       </c>
-      <c r="G7" t="s" s="271">
+      <c r="H7" t="s" s="271">
+        <v>606</v>
+      </c>
+      <c r="I7" t="s" s="272">
         <v>607</v>
       </c>
-      <c r="H7" t="s" s="271">
+      <c r="J7" t="s" s="272">
+        <v>606</v>
+      </c>
+      <c r="K7" t="s" s="273">
         <v>608</v>
       </c>
-      <c r="I7" t="s" s="272">
+      <c r="L7" t="s" s="273">
+        <v>606</v>
+      </c>
+      <c r="M7" t="s" s="274">
         <v>609</v>
       </c>
-      <c r="J7" t="s" s="272">
-        <v>608</v>
-      </c>
-      <c r="K7" t="s" s="273">
-        <v>610</v>
-      </c>
-      <c r="L7" t="s" s="273">
-        <v>608</v>
-      </c>
-      <c r="M7" t="s" s="274">
+      <c r="N7" t="s" s="274">
+        <v>606</v>
+      </c>
+      <c r="O7" t="s" s="275">
+        <v>618</v>
+      </c>
+      <c r="P7" t="s" s="275">
+        <v>606</v>
+      </c>
+      <c r="Q7" t="s" s="276">
         <v>611</v>
       </c>
-      <c r="N7" t="s" s="274">
-        <v>608</v>
-      </c>
-      <c r="O7" t="s" s="275">
-        <v>620</v>
-      </c>
-      <c r="P7" t="s" s="275">
-        <v>608</v>
-      </c>
-      <c r="Q7" t="s" s="276">
-        <v>613</v>
-      </c>
       <c r="R7" t="s" s="276">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="S7" t="s" s="277">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="T7" t="s" s="277">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C8" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D8" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="E8" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="F8" t="s">
+        <v>614</v>
+      </c>
+      <c r="G8" t="s" s="278">
+        <v>605</v>
+      </c>
+      <c r="H8" t="s" s="278">
+        <v>606</v>
+      </c>
+      <c r="I8" t="s" s="279">
+        <v>607</v>
+      </c>
+      <c r="J8" t="s" s="279">
+        <v>606</v>
+      </c>
+      <c r="K8" t="s" s="280">
+        <v>608</v>
+      </c>
+      <c r="L8" t="s" s="280">
+        <v>606</v>
+      </c>
+      <c r="M8" t="s" s="281">
+        <v>609</v>
+      </c>
+      <c r="N8" t="s" s="281">
+        <v>606</v>
+      </c>
+      <c r="O8" t="s" s="282">
+        <v>618</v>
+      </c>
+      <c r="P8" t="s" s="282">
+        <v>606</v>
+      </c>
+      <c r="Q8" t="s" s="283">
+        <v>615</v>
+      </c>
+      <c r="R8" t="s" s="283">
+        <v>606</v>
+      </c>
+      <c r="S8" t="s" s="284">
         <v>616</v>
       </c>
-      <c r="G8" t="s" s="278">
-        <v>607</v>
-      </c>
-      <c r="H8" t="s" s="278">
-        <v>608</v>
-      </c>
-      <c r="I8" t="s" s="279">
-        <v>609</v>
-      </c>
-      <c r="J8" t="s" s="279">
-        <v>608</v>
-      </c>
-      <c r="K8" t="s" s="280">
-        <v>610</v>
-      </c>
-      <c r="L8" t="s" s="280">
-        <v>608</v>
-      </c>
-      <c r="M8" t="s" s="281">
-        <v>611</v>
-      </c>
-      <c r="N8" t="s" s="281">
-        <v>608</v>
-      </c>
-      <c r="O8" t="s" s="282">
-        <v>620</v>
-      </c>
-      <c r="P8" t="s" s="282">
-        <v>608</v>
-      </c>
-      <c r="Q8" t="s" s="283">
-        <v>617</v>
-      </c>
-      <c r="R8" t="s" s="283">
-        <v>608</v>
-      </c>
-      <c r="S8" t="s" s="284">
-        <v>618</v>
-      </c>
       <c r="T8" t="s" s="284">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C10" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D10" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="E10" t="s">
+        <v>619</v>
+      </c>
+      <c r="F10" t="s">
+        <v>603</v>
+      </c>
+      <c r="G10" t="s" s="285">
+        <v>605</v>
+      </c>
+      <c r="H10" t="s" s="285">
+        <v>606</v>
+      </c>
+      <c r="I10" t="s" s="286">
+        <v>607</v>
+      </c>
+      <c r="J10" t="s" s="286">
+        <v>606</v>
+      </c>
+      <c r="K10" t="s" s="287">
+        <v>608</v>
+      </c>
+      <c r="L10" t="s" s="287">
+        <v>606</v>
+      </c>
+      <c r="M10" t="s" s="288">
+        <v>609</v>
+      </c>
+      <c r="N10" t="s" s="288">
+        <v>606</v>
+      </c>
+      <c r="O10" t="s" s="289">
+        <v>620</v>
+      </c>
+      <c r="P10" t="s" s="289">
+        <v>606</v>
+      </c>
+      <c r="Q10" t="s" s="290">
+        <v>611</v>
+      </c>
+      <c r="R10" t="s" s="290">
+        <v>606</v>
+      </c>
+      <c r="S10" t="s" s="291">
         <v>621</v>
       </c>
-      <c r="F10" t="s">
-        <v>605</v>
-      </c>
-      <c r="G10" t="s" s="285">
-        <v>607</v>
-      </c>
-      <c r="H10" t="s" s="285">
-        <v>608</v>
-      </c>
-      <c r="I10" t="s" s="286">
-        <v>609</v>
-      </c>
-      <c r="J10" t="s" s="286">
-        <v>608</v>
-      </c>
-      <c r="K10" t="s" s="287">
-        <v>610</v>
-      </c>
-      <c r="L10" t="s" s="287">
-        <v>608</v>
-      </c>
-      <c r="M10" t="s" s="288">
-        <v>611</v>
-      </c>
-      <c r="N10" t="s" s="288">
-        <v>608</v>
-      </c>
-      <c r="O10" t="s" s="289">
-        <v>622</v>
-      </c>
-      <c r="P10" t="s" s="289">
-        <v>608</v>
-      </c>
-      <c r="Q10" t="s" s="290">
-        <v>613</v>
-      </c>
-      <c r="R10" t="s" s="290">
-        <v>608</v>
-      </c>
-      <c r="S10" t="s" s="291">
-        <v>623</v>
-      </c>
       <c r="T10" t="s" s="291">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C11" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D11" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="E11" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="F11" t="s">
+        <v>614</v>
+      </c>
+      <c r="G11" t="s" s="292">
+        <v>605</v>
+      </c>
+      <c r="H11" t="s" s="292">
+        <v>606</v>
+      </c>
+      <c r="I11" t="s" s="293">
+        <v>607</v>
+      </c>
+      <c r="J11" t="s" s="293">
+        <v>606</v>
+      </c>
+      <c r="K11" t="s" s="294">
+        <v>608</v>
+      </c>
+      <c r="L11" t="s" s="294">
+        <v>606</v>
+      </c>
+      <c r="M11" t="s" s="295">
+        <v>609</v>
+      </c>
+      <c r="N11" t="s" s="295">
+        <v>606</v>
+      </c>
+      <c r="O11" t="s" s="296">
+        <v>620</v>
+      </c>
+      <c r="P11" t="s" s="296">
+        <v>606</v>
+      </c>
+      <c r="Q11" t="s" s="297">
+        <v>615</v>
+      </c>
+      <c r="R11" t="s" s="297">
+        <v>606</v>
+      </c>
+      <c r="S11" t="s" s="298">
         <v>616</v>
       </c>
-      <c r="G11" t="s" s="292">
-        <v>607</v>
-      </c>
-      <c r="H11" t="s" s="292">
-        <v>608</v>
-      </c>
-      <c r="I11" t="s" s="293">
-        <v>609</v>
-      </c>
-      <c r="J11" t="s" s="293">
-        <v>608</v>
-      </c>
-      <c r="K11" t="s" s="294">
-        <v>610</v>
-      </c>
-      <c r="L11" t="s" s="294">
-        <v>608</v>
-      </c>
-      <c r="M11" t="s" s="295">
-        <v>611</v>
-      </c>
-      <c r="N11" t="s" s="295">
-        <v>608</v>
-      </c>
-      <c r="O11" t="s" s="296">
-        <v>622</v>
-      </c>
-      <c r="P11" t="s" s="296">
-        <v>608</v>
-      </c>
-      <c r="Q11" t="s" s="297">
-        <v>617</v>
-      </c>
-      <c r="R11" t="s" s="297">
-        <v>608</v>
-      </c>
-      <c r="S11" t="s" s="298">
-        <v>618</v>
-      </c>
       <c r="T11" t="s" s="298">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C13" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D13" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="E13" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="F13" t="s">
+        <v>603</v>
+      </c>
+      <c r="G13" t="s" s="299">
         <v>605</v>
       </c>
-      <c r="G13" t="s" s="299">
+      <c r="H13" t="s" s="299">
+        <v>606</v>
+      </c>
+      <c r="I13" t="s" s="300">
         <v>607</v>
       </c>
-      <c r="H13" t="s" s="299">
+      <c r="J13" t="s" s="300">
+        <v>606</v>
+      </c>
+      <c r="K13" t="s" s="301">
         <v>608</v>
       </c>
-      <c r="I13" t="s" s="300">
+      <c r="L13" t="s" s="301">
+        <v>606</v>
+      </c>
+      <c r="M13" t="s" s="302">
         <v>609</v>
       </c>
-      <c r="J13" t="s" s="300">
-        <v>608</v>
-      </c>
-      <c r="K13" t="s" s="301">
-        <v>610</v>
-      </c>
-      <c r="L13" t="s" s="301">
-        <v>608</v>
-      </c>
-      <c r="M13" t="s" s="302">
+      <c r="N13" t="s" s="302">
+        <v>606</v>
+      </c>
+      <c r="O13" t="s" s="303">
+        <v>623</v>
+      </c>
+      <c r="P13" t="s" s="303">
+        <v>606</v>
+      </c>
+      <c r="Q13" t="s" s="304">
         <v>611</v>
       </c>
-      <c r="N13" t="s" s="302">
-        <v>608</v>
-      </c>
-      <c r="O13" t="s" s="303">
-        <v>625</v>
-      </c>
-      <c r="P13" t="s" s="303">
-        <v>608</v>
-      </c>
-      <c r="Q13" t="s" s="304">
-        <v>613</v>
-      </c>
       <c r="R13" t="s" s="304">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="S13" t="s" s="305">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="T13" t="s" s="305">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C14" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D14" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="E14" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="F14" t="s">
+        <v>614</v>
+      </c>
+      <c r="G14" t="s" s="306">
+        <v>605</v>
+      </c>
+      <c r="H14" t="s" s="306">
+        <v>606</v>
+      </c>
+      <c r="I14" t="s" s="307">
+        <v>607</v>
+      </c>
+      <c r="J14" t="s" s="307">
+        <v>606</v>
+      </c>
+      <c r="K14" t="s" s="308">
+        <v>608</v>
+      </c>
+      <c r="L14" t="s" s="308">
+        <v>606</v>
+      </c>
+      <c r="M14" t="s" s="309">
+        <v>609</v>
+      </c>
+      <c r="N14" t="s" s="309">
+        <v>606</v>
+      </c>
+      <c r="O14" t="s" s="310">
+        <v>623</v>
+      </c>
+      <c r="P14" t="s" s="310">
+        <v>606</v>
+      </c>
+      <c r="Q14" t="s" s="311">
+        <v>615</v>
+      </c>
+      <c r="R14" t="s" s="311">
+        <v>606</v>
+      </c>
+      <c r="S14" t="s" s="312">
         <v>616</v>
       </c>
-      <c r="G14" t="s" s="306">
-        <v>607</v>
-      </c>
-      <c r="H14" t="s" s="306">
-        <v>608</v>
-      </c>
-      <c r="I14" t="s" s="307">
-        <v>609</v>
-      </c>
-      <c r="J14" t="s" s="307">
-        <v>608</v>
-      </c>
-      <c r="K14" t="s" s="308">
-        <v>610</v>
-      </c>
-      <c r="L14" t="s" s="308">
-        <v>608</v>
-      </c>
-      <c r="M14" t="s" s="309">
-        <v>611</v>
-      </c>
-      <c r="N14" t="s" s="309">
-        <v>608</v>
-      </c>
-      <c r="O14" t="s" s="310">
-        <v>625</v>
-      </c>
-      <c r="P14" t="s" s="310">
-        <v>608</v>
-      </c>
-      <c r="Q14" t="s" s="311">
-        <v>617</v>
-      </c>
-      <c r="R14" t="s" s="311">
-        <v>608</v>
-      </c>
-      <c r="S14" t="s" s="312">
-        <v>618</v>
-      </c>
       <c r="T14" t="s" s="312">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
+        <v>599</v>
+      </c>
+      <c r="C16" t="s">
+        <v>602</v>
+      </c>
+      <c r="D16" t="s">
+        <v>624</v>
+      </c>
+      <c r="E16" t="s">
         <v>601</v>
       </c>
-      <c r="C16" t="s">
-        <v>604</v>
-      </c>
-      <c r="D16" t="s">
-        <v>626</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>603</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s" s="313">
         <v>605</v>
       </c>
-      <c r="G16" t="s" s="313">
+      <c r="H16" t="s" s="313">
+        <v>606</v>
+      </c>
+      <c r="I16" t="s" s="314">
         <v>607</v>
       </c>
-      <c r="H16" t="s" s="313">
-        <v>608</v>
-      </c>
-      <c r="I16" t="s" s="314">
+      <c r="J16" t="s" s="314">
+        <v>606</v>
+      </c>
+      <c r="K16" t="s" s="315">
+        <v>625</v>
+      </c>
+      <c r="L16" t="s" s="315">
+        <v>606</v>
+      </c>
+      <c r="M16" t="s" s="316">
         <v>609</v>
       </c>
-      <c r="J16" t="s" s="314">
-        <v>608</v>
-      </c>
-      <c r="K16" t="s" s="315">
-        <v>627</v>
-      </c>
-      <c r="L16" t="s" s="315">
-        <v>608</v>
-      </c>
-      <c r="M16" t="s" s="316">
+      <c r="N16" t="s" s="316">
+        <v>606</v>
+      </c>
+      <c r="O16" t="s" s="317">
+        <v>610</v>
+      </c>
+      <c r="P16" t="s" s="317">
+        <v>606</v>
+      </c>
+      <c r="Q16" t="s" s="318">
         <v>611</v>
       </c>
-      <c r="N16" t="s" s="316">
-        <v>608</v>
-      </c>
-      <c r="O16" t="s" s="317">
+      <c r="R16" t="s" s="318">
+        <v>606</v>
+      </c>
+      <c r="S16" t="s" s="319">
         <v>612</v>
       </c>
-      <c r="P16" t="s" s="317">
-        <v>608</v>
-      </c>
-      <c r="Q16" t="s" s="318">
-        <v>613</v>
-      </c>
-      <c r="R16" t="s" s="318">
-        <v>608</v>
-      </c>
-      <c r="S16" t="s" s="319">
-        <v>614</v>
-      </c>
       <c r="T16" t="s" s="319">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
+        <v>599</v>
+      </c>
+      <c r="C17" t="s">
+        <v>602</v>
+      </c>
+      <c r="D17" t="s">
+        <v>624</v>
+      </c>
+      <c r="E17" t="s">
         <v>601</v>
       </c>
-      <c r="C17" t="s">
-        <v>604</v>
-      </c>
-      <c r="D17" t="s">
-        <v>626</v>
-      </c>
-      <c r="E17" t="s">
-        <v>603</v>
-      </c>
       <c r="F17" t="s">
+        <v>614</v>
+      </c>
+      <c r="G17" t="s" s="320">
+        <v>605</v>
+      </c>
+      <c r="H17" t="s" s="320">
+        <v>606</v>
+      </c>
+      <c r="I17" t="s" s="321">
+        <v>607</v>
+      </c>
+      <c r="J17" t="s" s="321">
+        <v>606</v>
+      </c>
+      <c r="K17" t="s" s="322">
+        <v>625</v>
+      </c>
+      <c r="L17" t="s" s="322">
+        <v>606</v>
+      </c>
+      <c r="M17" t="s" s="323">
+        <v>609</v>
+      </c>
+      <c r="N17" t="s" s="323">
+        <v>606</v>
+      </c>
+      <c r="O17" t="s" s="324">
+        <v>610</v>
+      </c>
+      <c r="P17" t="s" s="324">
+        <v>606</v>
+      </c>
+      <c r="Q17" t="s" s="325">
+        <v>615</v>
+      </c>
+      <c r="R17" t="s" s="325">
+        <v>606</v>
+      </c>
+      <c r="S17" t="s" s="326">
         <v>616</v>
       </c>
-      <c r="G17" t="s" s="320">
-        <v>607</v>
-      </c>
-      <c r="H17" t="s" s="320">
-        <v>608</v>
-      </c>
-      <c r="I17" t="s" s="321">
-        <v>609</v>
-      </c>
-      <c r="J17" t="s" s="321">
-        <v>608</v>
-      </c>
-      <c r="K17" t="s" s="322">
-        <v>627</v>
-      </c>
-      <c r="L17" t="s" s="322">
-        <v>608</v>
-      </c>
-      <c r="M17" t="s" s="323">
-        <v>611</v>
-      </c>
-      <c r="N17" t="s" s="323">
-        <v>608</v>
-      </c>
-      <c r="O17" t="s" s="324">
-        <v>612</v>
-      </c>
-      <c r="P17" t="s" s="324">
-        <v>608</v>
-      </c>
-      <c r="Q17" t="s" s="325">
-        <v>617</v>
-      </c>
-      <c r="R17" t="s" s="325">
-        <v>608</v>
-      </c>
-      <c r="S17" t="s" s="326">
-        <v>618</v>
-      </c>
       <c r="T17" t="s" s="326">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C19" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D19" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="E19" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="F19" t="s">
+        <v>603</v>
+      </c>
+      <c r="G19" t="s" s="327">
         <v>605</v>
       </c>
-      <c r="G19" t="s" s="327">
+      <c r="H19" t="s" s="327">
+        <v>606</v>
+      </c>
+      <c r="I19" t="s" s="328">
         <v>607</v>
       </c>
-      <c r="H19" t="s" s="327">
-        <v>608</v>
-      </c>
-      <c r="I19" t="s" s="328">
+      <c r="J19" t="s" s="328">
+        <v>606</v>
+      </c>
+      <c r="K19" t="s" s="329">
+        <v>625</v>
+      </c>
+      <c r="L19" t="s" s="329">
+        <v>606</v>
+      </c>
+      <c r="M19" t="s" s="330">
         <v>609</v>
       </c>
-      <c r="J19" t="s" s="328">
-        <v>608</v>
-      </c>
-      <c r="K19" t="s" s="329">
-        <v>627</v>
-      </c>
-      <c r="L19" t="s" s="329">
-        <v>608</v>
-      </c>
-      <c r="M19" t="s" s="330">
+      <c r="N19" t="s" s="330">
+        <v>606</v>
+      </c>
+      <c r="O19" t="s" s="331">
+        <v>618</v>
+      </c>
+      <c r="P19" t="s" s="331">
+        <v>606</v>
+      </c>
+      <c r="Q19" t="s" s="332">
         <v>611</v>
       </c>
-      <c r="N19" t="s" s="330">
-        <v>608</v>
-      </c>
-      <c r="O19" t="s" s="331">
-        <v>620</v>
-      </c>
-      <c r="P19" t="s" s="331">
-        <v>608</v>
-      </c>
-      <c r="Q19" t="s" s="332">
-        <v>613</v>
-      </c>
       <c r="R19" t="s" s="332">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="S19" t="s" s="333">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="T19" t="s" s="333">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C20" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D20" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="E20" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="F20" t="s">
+        <v>614</v>
+      </c>
+      <c r="G20" t="s" s="334">
+        <v>605</v>
+      </c>
+      <c r="H20" t="s" s="334">
+        <v>606</v>
+      </c>
+      <c r="I20" t="s" s="335">
+        <v>607</v>
+      </c>
+      <c r="J20" t="s" s="335">
+        <v>606</v>
+      </c>
+      <c r="K20" t="s" s="336">
+        <v>625</v>
+      </c>
+      <c r="L20" t="s" s="336">
+        <v>606</v>
+      </c>
+      <c r="M20" t="s" s="337">
+        <v>609</v>
+      </c>
+      <c r="N20" t="s" s="337">
+        <v>606</v>
+      </c>
+      <c r="O20" t="s" s="338">
+        <v>618</v>
+      </c>
+      <c r="P20" t="s" s="338">
+        <v>606</v>
+      </c>
+      <c r="Q20" t="s" s="339">
+        <v>615</v>
+      </c>
+      <c r="R20" t="s" s="339">
+        <v>606</v>
+      </c>
+      <c r="S20" t="s" s="340">
         <v>616</v>
       </c>
-      <c r="G20" t="s" s="334">
-        <v>607</v>
-      </c>
-      <c r="H20" t="s" s="334">
-        <v>608</v>
-      </c>
-      <c r="I20" t="s" s="335">
-        <v>609</v>
-      </c>
-      <c r="J20" t="s" s="335">
-        <v>608</v>
-      </c>
-      <c r="K20" t="s" s="336">
-        <v>627</v>
-      </c>
-      <c r="L20" t="s" s="336">
-        <v>608</v>
-      </c>
-      <c r="M20" t="s" s="337">
-        <v>611</v>
-      </c>
-      <c r="N20" t="s" s="337">
-        <v>608</v>
-      </c>
-      <c r="O20" t="s" s="338">
-        <v>620</v>
-      </c>
-      <c r="P20" t="s" s="338">
-        <v>608</v>
-      </c>
-      <c r="Q20" t="s" s="339">
-        <v>617</v>
-      </c>
-      <c r="R20" t="s" s="339">
-        <v>608</v>
-      </c>
-      <c r="S20" t="s" s="340">
-        <v>618</v>
-      </c>
       <c r="T20" t="s" s="340">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C22" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D22" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="E22" t="s">
+        <v>619</v>
+      </c>
+      <c r="F22" t="s">
+        <v>603</v>
+      </c>
+      <c r="G22" t="s" s="341">
+        <v>605</v>
+      </c>
+      <c r="H22" t="s" s="341">
+        <v>606</v>
+      </c>
+      <c r="I22" t="s" s="342">
+        <v>607</v>
+      </c>
+      <c r="J22" t="s" s="342">
+        <v>606</v>
+      </c>
+      <c r="K22" t="s" s="343">
+        <v>625</v>
+      </c>
+      <c r="L22" t="s" s="343">
+        <v>606</v>
+      </c>
+      <c r="M22" t="s" s="344">
+        <v>609</v>
+      </c>
+      <c r="N22" t="s" s="344">
+        <v>606</v>
+      </c>
+      <c r="O22" t="s" s="345">
+        <v>620</v>
+      </c>
+      <c r="P22" t="s" s="345">
+        <v>606</v>
+      </c>
+      <c r="Q22" t="s" s="346">
+        <v>611</v>
+      </c>
+      <c r="R22" t="s" s="346">
+        <v>606</v>
+      </c>
+      <c r="S22" t="s" s="347">
         <v>621</v>
       </c>
-      <c r="F22" t="s">
-        <v>605</v>
-      </c>
-      <c r="G22" t="s" s="341">
-        <v>607</v>
-      </c>
-      <c r="H22" t="s" s="341">
-        <v>608</v>
-      </c>
-      <c r="I22" t="s" s="342">
-        <v>609</v>
-      </c>
-      <c r="J22" t="s" s="342">
-        <v>608</v>
-      </c>
-      <c r="K22" t="s" s="343">
-        <v>627</v>
-      </c>
-      <c r="L22" t="s" s="343">
-        <v>608</v>
-      </c>
-      <c r="M22" t="s" s="344">
-        <v>611</v>
-      </c>
-      <c r="N22" t="s" s="344">
-        <v>608</v>
-      </c>
-      <c r="O22" t="s" s="345">
-        <v>622</v>
-      </c>
-      <c r="P22" t="s" s="345">
-        <v>608</v>
-      </c>
-      <c r="Q22" t="s" s="346">
-        <v>613</v>
-      </c>
-      <c r="R22" t="s" s="346">
-        <v>608</v>
-      </c>
-      <c r="S22" t="s" s="347">
-        <v>623</v>
-      </c>
       <c r="T22" t="s" s="347">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C23" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D23" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="E23" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="F23" t="s">
+        <v>614</v>
+      </c>
+      <c r="G23" t="s" s="348">
+        <v>605</v>
+      </c>
+      <c r="H23" t="s" s="348">
+        <v>606</v>
+      </c>
+      <c r="I23" t="s" s="349">
+        <v>607</v>
+      </c>
+      <c r="J23" t="s" s="349">
+        <v>606</v>
+      </c>
+      <c r="K23" t="s" s="350">
+        <v>625</v>
+      </c>
+      <c r="L23" t="s" s="350">
+        <v>606</v>
+      </c>
+      <c r="M23" t="s" s="351">
+        <v>609</v>
+      </c>
+      <c r="N23" t="s" s="351">
+        <v>606</v>
+      </c>
+      <c r="O23" t="s" s="352">
+        <v>620</v>
+      </c>
+      <c r="P23" t="s" s="352">
+        <v>606</v>
+      </c>
+      <c r="Q23" t="s" s="353">
+        <v>615</v>
+      </c>
+      <c r="R23" t="s" s="353">
+        <v>606</v>
+      </c>
+      <c r="S23" t="s" s="354">
         <v>616</v>
       </c>
-      <c r="G23" t="s" s="348">
-        <v>607</v>
-      </c>
-      <c r="H23" t="s" s="348">
-        <v>608</v>
-      </c>
-      <c r="I23" t="s" s="349">
-        <v>609</v>
-      </c>
-      <c r="J23" t="s" s="349">
-        <v>608</v>
-      </c>
-      <c r="K23" t="s" s="350">
-        <v>627</v>
-      </c>
-      <c r="L23" t="s" s="350">
-        <v>608</v>
-      </c>
-      <c r="M23" t="s" s="351">
-        <v>611</v>
-      </c>
-      <c r="N23" t="s" s="351">
-        <v>608</v>
-      </c>
-      <c r="O23" t="s" s="352">
-        <v>622</v>
-      </c>
-      <c r="P23" t="s" s="352">
-        <v>608</v>
-      </c>
-      <c r="Q23" t="s" s="353">
-        <v>617</v>
-      </c>
-      <c r="R23" t="s" s="353">
-        <v>608</v>
-      </c>
-      <c r="S23" t="s" s="354">
-        <v>618</v>
-      </c>
       <c r="T23" t="s" s="354">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C25" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D25" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="E25" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="F25" t="s">
+        <v>603</v>
+      </c>
+      <c r="G25" t="s" s="355">
         <v>605</v>
       </c>
-      <c r="G25" t="s" s="355">
+      <c r="H25" t="s" s="355">
+        <v>606</v>
+      </c>
+      <c r="I25" t="s" s="356">
         <v>607</v>
       </c>
-      <c r="H25" t="s" s="355">
-        <v>608</v>
-      </c>
-      <c r="I25" t="s" s="356">
+      <c r="J25" t="s" s="356">
+        <v>606</v>
+      </c>
+      <c r="K25" t="s" s="357">
+        <v>625</v>
+      </c>
+      <c r="L25" t="s" s="357">
+        <v>606</v>
+      </c>
+      <c r="M25" t="s" s="358">
         <v>609</v>
       </c>
-      <c r="J25" t="s" s="356">
-        <v>608</v>
-      </c>
-      <c r="K25" t="s" s="357">
-        <v>627</v>
-      </c>
-      <c r="L25" t="s" s="357">
-        <v>608</v>
-      </c>
-      <c r="M25" t="s" s="358">
+      <c r="N25" t="s" s="358">
+        <v>606</v>
+      </c>
+      <c r="O25" t="s" s="359">
+        <v>623</v>
+      </c>
+      <c r="P25" t="s" s="359">
+        <v>606</v>
+      </c>
+      <c r="Q25" t="s" s="360">
         <v>611</v>
       </c>
-      <c r="N25" t="s" s="358">
-        <v>608</v>
-      </c>
-      <c r="O25" t="s" s="359">
-        <v>625</v>
-      </c>
-      <c r="P25" t="s" s="359">
-        <v>608</v>
-      </c>
-      <c r="Q25" t="s" s="360">
-        <v>613</v>
-      </c>
       <c r="R25" t="s" s="360">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="S25" t="s" s="361">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="T25" t="s" s="361">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C26" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D26" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="E26" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="F26" t="s">
+        <v>614</v>
+      </c>
+      <c r="G26" t="s" s="362">
+        <v>605</v>
+      </c>
+      <c r="H26" t="s" s="362">
+        <v>606</v>
+      </c>
+      <c r="I26" t="s" s="363">
+        <v>607</v>
+      </c>
+      <c r="J26" t="s" s="363">
+        <v>606</v>
+      </c>
+      <c r="K26" t="s" s="364">
+        <v>625</v>
+      </c>
+      <c r="L26" t="s" s="364">
+        <v>606</v>
+      </c>
+      <c r="M26" t="s" s="365">
+        <v>609</v>
+      </c>
+      <c r="N26" t="s" s="365">
+        <v>606</v>
+      </c>
+      <c r="O26" t="s" s="366">
+        <v>623</v>
+      </c>
+      <c r="P26" t="s" s="366">
+        <v>606</v>
+      </c>
+      <c r="Q26" t="s" s="367">
+        <v>615</v>
+      </c>
+      <c r="R26" t="s" s="367">
+        <v>606</v>
+      </c>
+      <c r="S26" t="s" s="368">
         <v>616</v>
       </c>
-      <c r="G26" t="s" s="362">
-        <v>607</v>
-      </c>
-      <c r="H26" t="s" s="362">
-        <v>608</v>
-      </c>
-      <c r="I26" t="s" s="363">
-        <v>609</v>
-      </c>
-      <c r="J26" t="s" s="363">
-        <v>608</v>
-      </c>
-      <c r="K26" t="s" s="364">
-        <v>627</v>
-      </c>
-      <c r="L26" t="s" s="364">
-        <v>608</v>
-      </c>
-      <c r="M26" t="s" s="365">
-        <v>611</v>
-      </c>
-      <c r="N26" t="s" s="365">
-        <v>608</v>
-      </c>
-      <c r="O26" t="s" s="366">
-        <v>625</v>
-      </c>
-      <c r="P26" t="s" s="366">
-        <v>608</v>
-      </c>
-      <c r="Q26" t="s" s="367">
-        <v>617</v>
-      </c>
-      <c r="R26" t="s" s="367">
-        <v>608</v>
-      </c>
-      <c r="S26" t="s" s="368">
-        <v>618</v>
-      </c>
       <c r="T26" t="s" s="368">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
+        <v>599</v>
+      </c>
+      <c r="C28" t="s">
+        <v>602</v>
+      </c>
+      <c r="D28" t="s">
+        <v>626</v>
+      </c>
+      <c r="E28" t="s">
         <v>601</v>
       </c>
-      <c r="C28" t="s">
-        <v>604</v>
-      </c>
-      <c r="D28" t="s">
-        <v>628</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>603</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s" s="369">
         <v>605</v>
       </c>
-      <c r="G28" t="s" s="369">
+      <c r="H28" t="s" s="369">
+        <v>606</v>
+      </c>
+      <c r="I28" t="s" s="370">
         <v>607</v>
       </c>
-      <c r="H28" t="s" s="369">
-        <v>608</v>
-      </c>
-      <c r="I28" t="s" s="370">
+      <c r="J28" t="s" s="370">
+        <v>606</v>
+      </c>
+      <c r="K28" t="s" s="371">
+        <v>627</v>
+      </c>
+      <c r="L28" t="s" s="371">
+        <v>606</v>
+      </c>
+      <c r="M28" t="s" s="372">
         <v>609</v>
       </c>
-      <c r="J28" t="s" s="370">
-        <v>608</v>
-      </c>
-      <c r="K28" t="s" s="371">
-        <v>629</v>
-      </c>
-      <c r="L28" t="s" s="371">
-        <v>608</v>
-      </c>
-      <c r="M28" t="s" s="372">
+      <c r="N28" t="s" s="372">
+        <v>606</v>
+      </c>
+      <c r="O28" t="s" s="373">
+        <v>610</v>
+      </c>
+      <c r="P28" t="s" s="373">
+        <v>606</v>
+      </c>
+      <c r="Q28" t="s" s="374">
         <v>611</v>
       </c>
-      <c r="N28" t="s" s="372">
-        <v>608</v>
-      </c>
-      <c r="O28" t="s" s="373">
+      <c r="R28" t="s" s="374">
+        <v>606</v>
+      </c>
+      <c r="S28" t="s" s="375">
         <v>612</v>
       </c>
-      <c r="P28" t="s" s="373">
-        <v>608</v>
-      </c>
-      <c r="Q28" t="s" s="374">
-        <v>613</v>
-      </c>
-      <c r="R28" t="s" s="374">
-        <v>608</v>
-      </c>
-      <c r="S28" t="s" s="375">
-        <v>614</v>
-      </c>
       <c r="T28" t="s" s="375">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
+        <v>599</v>
+      </c>
+      <c r="C29" t="s">
+        <v>602</v>
+      </c>
+      <c r="D29" t="s">
+        <v>626</v>
+      </c>
+      <c r="E29" t="s">
         <v>601</v>
       </c>
-      <c r="C29" t="s">
-        <v>604</v>
-      </c>
-      <c r="D29" t="s">
-        <v>628</v>
-      </c>
-      <c r="E29" t="s">
-        <v>603</v>
-      </c>
       <c r="F29" t="s">
+        <v>614</v>
+      </c>
+      <c r="G29" t="s" s="376">
+        <v>605</v>
+      </c>
+      <c r="H29" t="s" s="376">
+        <v>606</v>
+      </c>
+      <c r="I29" t="s" s="377">
+        <v>607</v>
+      </c>
+      <c r="J29" t="s" s="377">
+        <v>606</v>
+      </c>
+      <c r="K29" t="s" s="378">
+        <v>627</v>
+      </c>
+      <c r="L29" t="s" s="378">
+        <v>606</v>
+      </c>
+      <c r="M29" t="s" s="379">
+        <v>609</v>
+      </c>
+      <c r="N29" t="s" s="379">
+        <v>606</v>
+      </c>
+      <c r="O29" t="s" s="380">
+        <v>610</v>
+      </c>
+      <c r="P29" t="s" s="380">
+        <v>606</v>
+      </c>
+      <c r="Q29" t="s" s="381">
+        <v>615</v>
+      </c>
+      <c r="R29" t="s" s="381">
+        <v>606</v>
+      </c>
+      <c r="S29" t="s" s="382">
         <v>616</v>
       </c>
-      <c r="G29" t="s" s="376">
-        <v>607</v>
-      </c>
-      <c r="H29" t="s" s="376">
-        <v>608</v>
-      </c>
-      <c r="I29" t="s" s="377">
-        <v>609</v>
-      </c>
-      <c r="J29" t="s" s="377">
-        <v>608</v>
-      </c>
-      <c r="K29" t="s" s="378">
-        <v>629</v>
-      </c>
-      <c r="L29" t="s" s="378">
-        <v>608</v>
-      </c>
-      <c r="M29" t="s" s="379">
-        <v>611</v>
-      </c>
-      <c r="N29" t="s" s="379">
-        <v>608</v>
-      </c>
-      <c r="O29" t="s" s="380">
-        <v>612</v>
-      </c>
-      <c r="P29" t="s" s="380">
-        <v>608</v>
-      </c>
-      <c r="Q29" t="s" s="381">
-        <v>617</v>
-      </c>
-      <c r="R29" t="s" s="381">
-        <v>608</v>
-      </c>
-      <c r="S29" t="s" s="382">
-        <v>618</v>
-      </c>
       <c r="T29" t="s" s="382">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C31" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D31" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="E31" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="F31" t="s">
+        <v>603</v>
+      </c>
+      <c r="G31" t="s" s="383">
         <v>605</v>
       </c>
-      <c r="G31" t="s" s="383">
+      <c r="H31" t="s" s="383">
+        <v>606</v>
+      </c>
+      <c r="I31" t="s" s="384">
         <v>607</v>
       </c>
-      <c r="H31" t="s" s="383">
-        <v>608</v>
-      </c>
-      <c r="I31" t="s" s="384">
+      <c r="J31" t="s" s="384">
+        <v>606</v>
+      </c>
+      <c r="K31" t="s" s="385">
+        <v>627</v>
+      </c>
+      <c r="L31" t="s" s="385">
+        <v>606</v>
+      </c>
+      <c r="M31" t="s" s="386">
         <v>609</v>
       </c>
-      <c r="J31" t="s" s="384">
-        <v>608</v>
-      </c>
-      <c r="K31" t="s" s="385">
-        <v>629</v>
-      </c>
-      <c r="L31" t="s" s="385">
-        <v>608</v>
-      </c>
-      <c r="M31" t="s" s="386">
+      <c r="N31" t="s" s="386">
+        <v>606</v>
+      </c>
+      <c r="O31" t="s" s="387">
+        <v>618</v>
+      </c>
+      <c r="P31" t="s" s="387">
+        <v>606</v>
+      </c>
+      <c r="Q31" t="s" s="388">
         <v>611</v>
       </c>
-      <c r="N31" t="s" s="386">
-        <v>608</v>
-      </c>
-      <c r="O31" t="s" s="387">
-        <v>620</v>
-      </c>
-      <c r="P31" t="s" s="387">
-        <v>608</v>
-      </c>
-      <c r="Q31" t="s" s="388">
-        <v>613</v>
-      </c>
       <c r="R31" t="s" s="388">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="S31" t="s" s="389">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="T31" t="s" s="389">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C32" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D32" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="E32" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="F32" t="s">
+        <v>614</v>
+      </c>
+      <c r="G32" t="s" s="390">
+        <v>605</v>
+      </c>
+      <c r="H32" t="s" s="390">
+        <v>606</v>
+      </c>
+      <c r="I32" t="s" s="391">
+        <v>607</v>
+      </c>
+      <c r="J32" t="s" s="391">
+        <v>606</v>
+      </c>
+      <c r="K32" t="s" s="392">
+        <v>627</v>
+      </c>
+      <c r="L32" t="s" s="392">
+        <v>606</v>
+      </c>
+      <c r="M32" t="s" s="393">
+        <v>609</v>
+      </c>
+      <c r="N32" t="s" s="393">
+        <v>606</v>
+      </c>
+      <c r="O32" t="s" s="394">
+        <v>618</v>
+      </c>
+      <c r="P32" t="s" s="394">
+        <v>606</v>
+      </c>
+      <c r="Q32" t="s" s="395">
+        <v>615</v>
+      </c>
+      <c r="R32" t="s" s="395">
+        <v>606</v>
+      </c>
+      <c r="S32" t="s" s="396">
         <v>616</v>
       </c>
-      <c r="G32" t="s" s="390">
-        <v>607</v>
-      </c>
-      <c r="H32" t="s" s="390">
-        <v>608</v>
-      </c>
-      <c r="I32" t="s" s="391">
-        <v>609</v>
-      </c>
-      <c r="J32" t="s" s="391">
-        <v>608</v>
-      </c>
-      <c r="K32" t="s" s="392">
-        <v>629</v>
-      </c>
-      <c r="L32" t="s" s="392">
-        <v>608</v>
-      </c>
-      <c r="M32" t="s" s="393">
-        <v>611</v>
-      </c>
-      <c r="N32" t="s" s="393">
-        <v>608</v>
-      </c>
-      <c r="O32" t="s" s="394">
-        <v>620</v>
-      </c>
-      <c r="P32" t="s" s="394">
-        <v>608</v>
-      </c>
-      <c r="Q32" t="s" s="395">
-        <v>617</v>
-      </c>
-      <c r="R32" t="s" s="395">
-        <v>608</v>
-      </c>
-      <c r="S32" t="s" s="396">
-        <v>618</v>
-      </c>
       <c r="T32" t="s" s="396">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
   </sheetData>

</xml_diff>